<commit_message>
login and signup improved
</commit_message>
<xml_diff>
--- a/Article Category Data/Categories2023-04-16 234936.426335.xlsx
+++ b/Article Category Data/Categories2023-04-16 234936.426335.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\Hadiya\fyp\khulasa\Article Category Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99519A31-D8CF-436B-B375-C0489466C3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="498" count="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="454">
   <si>
     <t>title</t>
   </si>
@@ -227,7 +235,7 @@
     <t>https://jang.com.pk/news/1216182</t>
   </si>
   <si>
-    <t>آزادکشمیر میں وزارت عظمیٰ کیلئے پارٹی میں اختلافات، پی ٹی آئی نام فائنل نہ کرسکی </t>
+    <t>آزادکشمیر میں وزارت عظمیٰ کیلئے پارٹی میں اختلافات، پی ٹی آئی نام فائنل نہ کرسکی</t>
   </si>
   <si>
     <t>https://jang.com.pk/news/1216180</t>
@@ -281,13 +289,13 @@
     <t>https://jang.com.pk/news/1216157</t>
   </si>
   <si>
-    <t>ن لیگ کی وزیراعظم آزاد کشمیر کیلئے امیدوار لانے پر مشاورت </t>
+    <t>ن لیگ کی وزیراعظم آزاد کشمیر کیلئے امیدوار لانے پر مشاورت</t>
   </si>
   <si>
     <t>https://jang.com.pk/news/1216184</t>
   </si>
   <si>
-    <t> آج پاکستان میں جو حالات ہیں اس کی وجہ کیا ہے؟ حنیف عباسی</t>
+    <t>آج پاکستان میں جو حالات ہیں اس کی وجہ کیا ہے؟ حنیف عباسی</t>
   </si>
   <si>
     <t>https://jang.com.pk/news/1216188</t>
@@ -305,7 +313,7 @@
     <t>https://jang.com.pk/news/1216174</t>
   </si>
   <si>
-    <t>وزیراعظم شہباز شریف چینی کی اسمگلنگ اور ناجائز منافع خوری پر برہم </t>
+    <t>وزیراعظم شہباز شریف چینی کی اسمگلنگ اور ناجائز منافع خوری پر برہم</t>
   </si>
   <si>
     <t>https://jang.com.pk/news/1216163</t>
@@ -353,7 +361,7 @@
     <t>https://jang.com.pk/news/1216170</t>
   </si>
   <si>
-    <t>ڈانس اور میں ایک دوسرے کے دشمن ہیں: فواد خان </t>
+    <t>ڈانس اور میں ایک دوسرے کے دشمن ہیں: فواد خان</t>
   </si>
   <si>
     <t>https://jang.com.pk/news/1216143</t>
@@ -485,19 +493,19 @@
     <t>https://jang.com.pk/news/1216004</t>
   </si>
   <si>
-    <t>اسٹیٹ بینک حکومت کے اکاؤنٹ سے کیسے پیسے لے سکتا ہے؟، مفتاح اسماعیل </t>
+    <t>اسٹیٹ بینک حکومت کے اکاؤنٹ سے کیسے پیسے لے سکتا ہے؟، مفتاح اسماعیل</t>
   </si>
   <si>
     <t>https://jang.com.pk/news/1216005</t>
   </si>
   <si>
-    <t>پاکستان مزید مالی یقین دہانی کرائے، آئی ایم ایف </t>
+    <t>پاکستان مزید مالی یقین دہانی کرائے، آئی ایم ایف</t>
   </si>
   <si>
     <t>https://jang.com.pk/news/1216006</t>
   </si>
   <si>
-    <t>’’عمران خان نے مجھے فون کرکے کہا تھا کہ میں امریکہ کا مخالف نہیں ہوں‘‘ </t>
+    <t>’’عمران خان نے مجھے فون کرکے کہا تھا کہ میں امریکہ کا مخالف نہیں ہوں‘‘</t>
   </si>
   <si>
     <t>https://jang.com.pk/news/1216007</t>
@@ -509,7 +517,7 @@
     <t>https://jang.com.pk/news/1216008</t>
   </si>
   <si>
-    <t>شرائط پوری، IMF کے پاس معاہدہ نہ کرنیکا کوئی بہانہ نہیں، وزیراعظم </t>
+    <t>شرائط پوری، IMF کے پاس معاہدہ نہ کرنیکا کوئی بہانہ نہیں، وزیراعظم</t>
   </si>
   <si>
     <t>https://jang.com.pk/news/1216010</t>
@@ -1103,7 +1111,7 @@
     <t>https://jang.com.pk/news/1215897</t>
   </si>
   <si>
-    <t>کاؤنٹی چیمپئن شپ میں محمد عباس کی پھر شاندار پرفارمنس </t>
+    <t>کاؤنٹی چیمپئن شپ میں محمد عباس کی پھر شاندار پرفارمنس</t>
   </si>
   <si>
     <t>https://jang.com.pk/news/1215896</t>
@@ -1250,7 +1258,7 @@
     <t>https://www.bbc.com/urdu/articles/cyx0zx4zdlgo</t>
   </si>
   <si>
-    <t>’میں اسے دیوار پر دے مارنا چاہتا ہوں‘: والدین کے ہاتھوں 10 ماہ کے بچے کا قتل جس نے جج کو بھی رلا دیا </t>
+    <t>’میں اسے دیوار پر دے مارنا چاہتا ہوں‘: والدین کے ہاتھوں 10 ماہ کے بچے کا قتل جس نے جج کو بھی رلا دیا</t>
   </si>
   <si>
     <t>https://www.bbc.com/urdu/articles/cn32mm78drno</t>
@@ -1374,147 +1382,15 @@
   </si>
   <si>
     <t>https://www.bbc.com/urdu/articles/ckv34pqw5zxo</t>
-  </si>
-  <si>
-    <t>’تری محفل میں لیکن ہم نہ ہوں گے‘</t>
-  </si>
-  <si>
-    <t>https://www.dawnnews.tv/news/1200152/</t>
-  </si>
-  <si>
-    <t>ایک فضائی میزبان کی آپ بیتی: عملہ اور فضا میں 13 ہزار گھنٹے</t>
-  </si>
-  <si>
-    <t>https://www.dawnnews.tv/news/1200455/</t>
-  </si>
-  <si>
-    <t>بہترین کیمرے کا حامل سستا ’رئیل می‘ نارزو متعارف</t>
-  </si>
-  <si>
-    <t>https://www.dawnnews.tv/news/1200778/</t>
-  </si>
-  <si>
-    <t>مکیش امبانی کے بیٹے کی سالگرہ میں عاطف اسلم اور راحت فتح علی خان نے سماں باندھ دیا</t>
-  </si>
-  <si>
-    <t>https://www.dawnnews.tv/news/1200756/</t>
-  </si>
-  <si>
-    <t>مفت آٹا، غریب عوام اور نااہل حکمراں</t>
-  </si>
-  <si>
-    <t>https://www.express.pk/story/2468363/464</t>
-  </si>
-  <si>
-    <t>ٹک ٹاک: پاکستان  سے اپ لوڈ ہونے والی 1 کروڑ 27 ہزار ویڈیوز ڈیلیٹ</t>
-  </si>
-  <si>
-    <t>https://www.jasarat.com/2023/04/13/tiktok-10/</t>
-  </si>
-  <si>
-    <t>’غیر مقبول‘ وزیراعظم سے مقبول اپوزیشن لیڈر تک: ’عمران خان کے بیانیے کی مقبولیت میں کلیدی کردار پی ڈی ایم کا رہا‘</t>
-  </si>
-  <si>
-    <t>https://www.bbc.com/urdu/articles/c72vg7xlwlwo</t>
-  </si>
-  <si>
-    <t>تاریخ پیدائش کی غلطی جس نے ایک نوجوان کو موت کے دہانے تک پہنچا دیا</t>
-  </si>
-  <si>
-    <t>https://www.bbc.com/urdu/articles/c2v34yd7743o</t>
-  </si>
-  <si>
-    <t>اسلامی ممالک میں بڑھتی قربتوں کے انڈیا پر کیا اثرات ہوں گے؟</t>
-  </si>
-  <si>
-    <t>https://www.bbc.com/urdu/articles/cd1785n9ynro</t>
-  </si>
-  <si>
-    <t>رونالڈو النصر کلب کے کوچ سے ’ناخوش‘: ’اب ٹیم کو رونالڈو کو ہی بطور کوچ رکھ لینا چاہیے‘</t>
-  </si>
-  <si>
-    <t>https://www.bbc.com/urdu/articles/cy7nww7pq8jo</t>
-  </si>
-  <si>
-    <t>چلو دلدار چلو، چاند کے پار چلو: مشتری کے چار چاندوں پر زندگی کے امکانات جاننے کا مشن</t>
-  </si>
-  <si>
-    <t>https://www.bbc.com/urdu/articles/c4nzjd8zxg0o</t>
-  </si>
-  <si>
-    <t>میانمار میں فوج کے فضائی حملے میں 80 سے زائد افراد ہلاک</t>
-  </si>
-  <si>
-    <t>https://www.dawnnews.tv/news/1200724/</t>
-  </si>
-  <si>
-    <t>رمضان المبارک میں اسرائیلی جارحیت</t>
-  </si>
-  <si>
-    <t>https://www.express.pk/story/2468242/464</t>
-  </si>
-  <si>
-    <t>پیشہ ورانہ خیانت</t>
-  </si>
-  <si>
-    <t>https://www.express.pk/story/2467738/464</t>
-  </si>
-  <si>
-    <t>کچھ ان کہی اور قدسیہ علی: ’بیٹا اچھی لگ رہی ہو، تھوڑا سا وزن کم کر لو تو اچھی جگہ رشتہ کروا دوں تمھارا‘</t>
-  </si>
-  <si>
-    <t>https://www.bbc.com/urdu/articles/cxwjdrggzv9o</t>
-  </si>
-  <si>
-    <t>عمران خان کی حکومت کے خاتمے کا ایک سال: سیاسی میدان میں کس نے  کیا کھویا اور  کیا پایا؟</t>
-  </si>
-  <si>
-    <t>https://www.bbc.com/urdu/articles/cmlzp8wkrweo</t>
-  </si>
-  <si>
-    <t>زبیدہ بنت جعفر: جب عباسی ملکہ نے لاکھوں دینار کی نہر بنوا کر کہا ’حساب قیامت کے دن پر چھوڑتی ہوں‘</t>
-  </si>
-  <si>
-    <t>https://www.bbc.com/urdu/articles/c2v31exl78no</t>
-  </si>
-  <si>
-    <t>’نور جہاں‘: کراچی چڑیا گھر کی بیمار ہتھنی ’تالاب میں گِرنے کے بعد سے پیروں پر کھڑی نہیں ہو پا رہی‘</t>
-  </si>
-  <si>
-    <t>https://www.bbc.com/urdu/articles/c04v91v219xo</t>
-  </si>
-  <si>
-    <t>گجرات میں احمدی ڈاکٹر کا قتل اور اُن کے مبینہ قاتل کی خودکشی کا معمہ جو سلجھنے کا نام نہیں لے رہا</t>
-  </si>
-  <si>
-    <t>https://www.bbc.com/urdu/articles/cd1y7qx1v0ko</t>
-  </si>
-  <si>
-    <t>خون آلود سیٹ پر ارشد شریف کے بال، گولیوں کی ٹائمنگ اور آئی فون: متضاد دعوے اور تحقیقات سے جڑے اہم  سوال</t>
-  </si>
-  <si>
-    <t>https://www.bbc.com/urdu/articles/cg3j3ngvv2jo</t>
-  </si>
-  <si>
-    <t>معاشرے میں خواتین کی تضحیک یعنی ’مساجنی‘ عام کیوں؟</t>
-  </si>
-  <si>
-    <t>https://www.bbc.com/urdu/articles/cy7n155dvppo</t>
-  </si>
-  <si>
-    <t>مصنوعی ذہانت: کیا اصلی اور نقلی کا فرق مٹ جائے گا؟</t>
-  </si>
-  <si>
-    <t>https://www.bbc.com/urdu/articles/cl5xel4p7e1o</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -1540,31 +1416,335 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C223"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="A223" sqref="A223"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.574285714285715" customWidth="1"/>
-    <col min="2" max="2" width="5.144285714285714" customWidth="1"/>
-    <col min="3" max="3" width="9.574285714285713" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1574,10 +1754,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1"/>
-      <c r="E1"/>
-    </row>
-    <row r="2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1588,7 +1766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1599,7 +1777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1610,7 +1788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1621,7 +1799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1632,7 +1810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1643,7 +1821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1654,7 +1832,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1665,7 +1843,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1676,7 +1854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1687,7 +1865,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1698,7 +1876,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1709,7 +1887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1720,7 +1898,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1731,7 +1909,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1742,7 +1920,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1753,7 +1931,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1764,7 +1942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1775,7 +1953,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1786,7 +1964,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -1797,7 +1975,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1808,7 +1986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -1819,7 +1997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -1830,7 +2008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1841,7 +2019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -1852,7 +2030,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1863,7 +2041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -1874,7 +2052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -1885,7 +2063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -1896,7 +2074,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -1907,7 +2085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -1918,7 +2096,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>73</v>
       </c>
@@ -1929,7 +2107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -1940,7 +2118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -1951,7 +2129,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -1962,7 +2140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -1973,7 +2151,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -1984,7 +2162,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>85</v>
       </c>
@@ -1995,7 +2173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>87</v>
       </c>
@@ -2006,7 +2184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>89</v>
       </c>
@@ -2017,7 +2195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>91</v>
       </c>
@@ -2028,7 +2206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>93</v>
       </c>
@@ -2039,7 +2217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -2050,7 +2228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>97</v>
       </c>
@@ -2061,7 +2239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>99</v>
       </c>
@@ -2072,7 +2250,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>101</v>
       </c>
@@ -2083,7 +2261,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>103</v>
       </c>
@@ -2094,7 +2272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>105</v>
       </c>
@@ -2105,7 +2283,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>107</v>
       </c>
@@ -2116,7 +2294,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>109</v>
       </c>
@@ -2127,7 +2305,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -2138,7 +2316,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>113</v>
       </c>
@@ -2149,7 +2327,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>115</v>
       </c>
@@ -2160,7 +2338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>117</v>
       </c>
@@ -2171,7 +2349,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>119</v>
       </c>
@@ -2182,7 +2360,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>121</v>
       </c>
@@ -2193,7 +2371,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>123</v>
       </c>
@@ -2204,7 +2382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>125</v>
       </c>
@@ -2215,7 +2393,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>127</v>
       </c>
@@ -2226,7 +2404,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>129</v>
       </c>
@@ -2237,7 +2415,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>131</v>
       </c>
@@ -2248,7 +2426,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>133</v>
       </c>
@@ -2259,7 +2437,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>135</v>
       </c>
@@ -2270,7 +2448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>137</v>
       </c>
@@ -2281,7 +2459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>139</v>
       </c>
@@ -2292,7 +2470,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>141</v>
       </c>
@@ -2303,7 +2481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>143</v>
       </c>
@@ -2314,7 +2492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>145</v>
       </c>
@@ -2325,7 +2503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>147</v>
       </c>
@@ -2336,7 +2514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -2347,7 +2525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>151</v>
       </c>
@@ -2358,7 +2536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>153</v>
       </c>
@@ -2369,7 +2547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>155</v>
       </c>
@@ -2380,7 +2558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>157</v>
       </c>
@@ -2391,7 +2569,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>159</v>
       </c>
@@ -2402,7 +2580,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>161</v>
       </c>
@@ -2413,7 +2591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>163</v>
       </c>
@@ -2424,7 +2602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>165</v>
       </c>
@@ -2435,7 +2613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>167</v>
       </c>
@@ -2446,7 +2624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>169</v>
       </c>
@@ -2457,7 +2635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>171</v>
       </c>
@@ -2468,7 +2646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>173</v>
       </c>
@@ -2479,7 +2657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>175</v>
       </c>
@@ -2490,7 +2668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>177</v>
       </c>
@@ -2501,7 +2679,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>179</v>
       </c>
@@ -2512,7 +2690,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>181</v>
       </c>
@@ -2523,7 +2701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>183</v>
       </c>
@@ -2534,7 +2712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>185</v>
       </c>
@@ -2545,7 +2723,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>187</v>
       </c>
@@ -2556,7 +2734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>189</v>
       </c>
@@ -2567,7 +2745,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>191</v>
       </c>
@@ -2578,7 +2756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>193</v>
       </c>
@@ -2589,7 +2767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>195</v>
       </c>
@@ -2600,7 +2778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>197</v>
       </c>
@@ -2611,7 +2789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>199</v>
       </c>
@@ -2622,7 +2800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>201</v>
       </c>
@@ -2633,7 +2811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>203</v>
       </c>
@@ -2644,7 +2822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>205</v>
       </c>
@@ -2655,7 +2833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>207</v>
       </c>
@@ -2666,7 +2844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>209</v>
       </c>
@@ -2677,7 +2855,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>211</v>
       </c>
@@ -2688,7 +2866,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>213</v>
       </c>
@@ -2699,7 +2877,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>215</v>
       </c>
@@ -2710,7 +2888,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>217</v>
       </c>
@@ -2721,7 +2899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>219</v>
       </c>
@@ -2732,7 +2910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>221</v>
       </c>
@@ -2743,7 +2921,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>223</v>
       </c>
@@ -2754,7 +2932,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>225</v>
       </c>
@@ -2765,7 +2943,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>227</v>
       </c>
@@ -2776,7 +2954,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>229</v>
       </c>
@@ -2787,7 +2965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>231</v>
       </c>
@@ -2798,7 +2976,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>233</v>
       </c>
@@ -2809,7 +2987,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>235</v>
       </c>
@@ -2820,7 +2998,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>237</v>
       </c>
@@ -2831,7 +3009,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>239</v>
       </c>
@@ -2842,7 +3020,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>241</v>
       </c>
@@ -2853,7 +3031,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>243</v>
       </c>
@@ -2864,7 +3042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>245</v>
       </c>
@@ -2875,7 +3053,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>247</v>
       </c>
@@ -2886,7 +3064,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>249</v>
       </c>
@@ -2897,7 +3075,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>251</v>
       </c>
@@ -2908,7 +3086,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>253</v>
       </c>
@@ -2919,7 +3097,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>255</v>
       </c>
@@ -2930,7 +3108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>257</v>
       </c>
@@ -2941,7 +3119,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>259</v>
       </c>
@@ -2952,7 +3130,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>261</v>
       </c>
@@ -2963,7 +3141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>263</v>
       </c>
@@ -2974,7 +3152,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>265</v>
       </c>
@@ -2985,7 +3163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>267</v>
       </c>
@@ -2996,7 +3174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>269</v>
       </c>
@@ -3007,7 +3185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>271</v>
       </c>
@@ -3018,7 +3196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>273</v>
       </c>
@@ -3029,7 +3207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>275</v>
       </c>
@@ -3040,7 +3218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>277</v>
       </c>
@@ -3051,7 +3229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>279</v>
       </c>
@@ -3062,7 +3240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>281</v>
       </c>
@@ -3073,7 +3251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>283</v>
       </c>
@@ -3084,7 +3262,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>285</v>
       </c>
@@ -3095,7 +3273,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>287</v>
       </c>
@@ -3106,7 +3284,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>289</v>
       </c>
@@ -3117,7 +3295,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>291</v>
       </c>
@@ -3128,7 +3306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>293</v>
       </c>
@@ -3139,7 +3317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>295</v>
       </c>
@@ -3150,7 +3328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>297</v>
       </c>
@@ -3161,7 +3339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>299</v>
       </c>
@@ -3172,7 +3350,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>301</v>
       </c>
@@ -3183,7 +3361,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>303</v>
       </c>
@@ -3194,7 +3372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>305</v>
       </c>
@@ -3205,7 +3383,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>307</v>
       </c>
@@ -3216,7 +3394,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>309</v>
       </c>
@@ -3227,7 +3405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>311</v>
       </c>
@@ -3238,7 +3416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>313</v>
       </c>
@@ -3249,7 +3427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>315</v>
       </c>
@@ -3260,7 +3438,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>317</v>
       </c>
@@ -3271,7 +3449,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>319</v>
       </c>
@@ -3282,7 +3460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>321</v>
       </c>
@@ -3293,7 +3471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>323</v>
       </c>
@@ -3304,7 +3482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>325</v>
       </c>
@@ -3315,7 +3493,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>327</v>
       </c>
@@ -3326,7 +3504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>329</v>
       </c>
@@ -3337,7 +3515,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>331</v>
       </c>
@@ -3348,7 +3526,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>333</v>
       </c>
@@ -3359,7 +3537,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>335</v>
       </c>
@@ -3370,7 +3548,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>337</v>
       </c>
@@ -3381,7 +3559,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>339</v>
       </c>
@@ -3392,7 +3570,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>341</v>
       </c>
@@ -3403,7 +3581,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>343</v>
       </c>
@@ -3414,7 +3592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>345</v>
       </c>
@@ -3425,7 +3603,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>347</v>
       </c>
@@ -3436,7 +3614,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>349</v>
       </c>
@@ -3447,7 +3625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>351</v>
       </c>
@@ -3458,7 +3636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>353</v>
       </c>
@@ -3469,7 +3647,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>355</v>
       </c>
@@ -3480,7 +3658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>357</v>
       </c>
@@ -3491,7 +3669,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>359</v>
       </c>
@@ -3502,7 +3680,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>361</v>
       </c>
@@ -3513,7 +3691,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>363</v>
       </c>
@@ -3524,7 +3702,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>365</v>
       </c>
@@ -3535,7 +3713,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>367</v>
       </c>
@@ -3546,7 +3724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>369</v>
       </c>
@@ -3557,7 +3735,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>371</v>
       </c>
@@ -3568,7 +3746,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>373</v>
       </c>
@@ -3579,7 +3757,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>375</v>
       </c>
@@ -3590,7 +3768,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>377</v>
       </c>
@@ -3601,7 +3779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>379</v>
       </c>
@@ -3612,7 +3790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>381</v>
       </c>
@@ -3623,7 +3801,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>383</v>
       </c>
@@ -3634,7 +3812,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>385</v>
       </c>
@@ -3645,7 +3823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>387</v>
       </c>
@@ -3656,7 +3834,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>389</v>
       </c>
@@ -3667,7 +3845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>391</v>
       </c>
@@ -3678,7 +3856,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>393</v>
       </c>
@@ -3689,7 +3867,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>395</v>
       </c>
@@ -3700,7 +3878,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>373</v>
       </c>
@@ -3711,7 +3889,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>398</v>
       </c>
@@ -3722,7 +3900,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>400</v>
       </c>
@@ -3733,7 +3911,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>402</v>
       </c>
@@ -3744,7 +3922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>404</v>
       </c>
@@ -3755,7 +3933,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>406</v>
       </c>
@@ -3766,7 +3944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>408</v>
       </c>
@@ -3777,7 +3955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>410</v>
       </c>
@@ -3788,7 +3966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>412</v>
       </c>
@@ -3799,7 +3977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>414</v>
       </c>
@@ -3810,7 +3988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>416</v>
       </c>
@@ -3821,7 +3999,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>418</v>
       </c>
@@ -3832,7 +4010,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>420</v>
       </c>
@@ -3843,7 +4021,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>422</v>
       </c>
@@ -3854,7 +4032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="209">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>424</v>
       </c>
@@ -3865,7 +4043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>426</v>
       </c>
@@ -3876,7 +4054,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>428</v>
       </c>
@@ -3887,7 +4065,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>430</v>
       </c>
@@ -3898,7 +4076,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>432</v>
       </c>
@@ -3909,7 +4087,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>434</v>
       </c>
@@ -3920,7 +4098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>436</v>
       </c>
@@ -3931,7 +4109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>438</v>
       </c>
@@ -3942,7 +4120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>440</v>
       </c>
@@ -3953,7 +4131,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="218">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>442</v>
       </c>
@@ -3964,7 +4142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>444</v>
       </c>
@@ -3975,7 +4153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>446</v>
       </c>
@@ -3986,7 +4164,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="221">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>448</v>
       </c>
@@ -3997,7 +4175,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="222">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>450</v>
       </c>
@@ -4008,7 +4186,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="223">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>452</v>
       </c>
@@ -4019,251 +4197,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="224">
-      <c r="A224" t="s">
-        <v>454</v>
-      </c>
-      <c r="B224" t="s">
-        <v>455</v>
-      </c>
-      <c r="C224" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="s">
-        <v>456</v>
-      </c>
-      <c r="B225" t="s">
-        <v>457</v>
-      </c>
-      <c r="C225" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="s">
-        <v>458</v>
-      </c>
-      <c r="B226" t="s">
-        <v>459</v>
-      </c>
-      <c r="C226" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="s">
-        <v>460</v>
-      </c>
-      <c r="B227" t="s">
-        <v>461</v>
-      </c>
-      <c r="C227" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="s">
-        <v>462</v>
-      </c>
-      <c r="B228" t="s">
-        <v>463</v>
-      </c>
-      <c r="C228" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="s">
-        <v>464</v>
-      </c>
-      <c r="B229" t="s">
-        <v>465</v>
-      </c>
-      <c r="C229" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="s">
-        <v>466</v>
-      </c>
-      <c r="B230" t="s">
-        <v>467</v>
-      </c>
-      <c r="C230" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="s">
-        <v>468</v>
-      </c>
-      <c r="B231" t="s">
-        <v>469</v>
-      </c>
-      <c r="C231" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="s">
-        <v>470</v>
-      </c>
-      <c r="B232" t="s">
-        <v>471</v>
-      </c>
-      <c r="C232" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="s">
-        <v>472</v>
-      </c>
-      <c r="B233" t="s">
-        <v>473</v>
-      </c>
-      <c r="C233" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" t="s">
-        <v>474</v>
-      </c>
-      <c r="B234" t="s">
-        <v>475</v>
-      </c>
-      <c r="C234" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" t="s">
-        <v>476</v>
-      </c>
-      <c r="B235" t="s">
-        <v>477</v>
-      </c>
-      <c r="C235" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" t="s">
-        <v>478</v>
-      </c>
-      <c r="B236" t="s">
-        <v>479</v>
-      </c>
-      <c r="C236" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" t="s">
-        <v>480</v>
-      </c>
-      <c r="B237" t="s">
-        <v>481</v>
-      </c>
-      <c r="C237" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" t="s">
-        <v>482</v>
-      </c>
-      <c r="B238" t="s">
-        <v>483</v>
-      </c>
-      <c r="C238" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" t="s">
-        <v>484</v>
-      </c>
-      <c r="B239" t="s">
-        <v>485</v>
-      </c>
-      <c r="C239" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" t="s">
-        <v>486</v>
-      </c>
-      <c r="B240" t="s">
-        <v>487</v>
-      </c>
-      <c r="C240" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" t="s">
-        <v>488</v>
-      </c>
-      <c r="B241" t="s">
-        <v>489</v>
-      </c>
-      <c r="C241" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" t="s">
-        <v>490</v>
-      </c>
-      <c r="B242" t="s">
-        <v>491</v>
-      </c>
-      <c r="C242" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" t="s">
-        <v>492</v>
-      </c>
-      <c r="B243" t="s">
-        <v>493</v>
-      </c>
-      <c r="C243" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" t="s">
-        <v>494</v>
-      </c>
-      <c r="B244" t="s">
-        <v>495</v>
-      </c>
-      <c r="C244" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" t="s">
-        <v>496</v>
-      </c>
-      <c r="B245" t="s">
-        <v>497</v>
-      </c>
-      <c r="C245" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1.0" bottom="1.0" header="0.5" footer="0.5"/>
-  <headerFooter scaleWithDoc="1" alignWithMargins="0" differentFirst="0" differentOddEven="0"/>
-  <extLst/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>